<commit_message>
changes related to batch cohort generation - WIP
</commit_message>
<xml_diff>
--- a/case studies/CaseStudy_TMDD/CaseStudy_TMDD_blank/Param_8.xlsx
+++ b/case studies/CaseStudy_TMDD/CaseStudy_TMDD_blank/Param_8.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hosseini/Desktop/Projects/TMDD Vpop/gQSPSim_Exp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feigelmj/Documents/Projects/gQSPsim/release/case studies/CaseStudy_TMDD/CaseStudy_TMDD_complete/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{39F39444-C023-314B-A379-15DECFA852EC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A721F44-6614-8842-93EC-360331FCAC20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="1860" windowWidth="25600" windowHeight="16920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>V1</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>s_target_init</t>
+  </si>
+  <si>
+    <t>Dist</t>
+  </si>
+  <si>
+    <t>norm</t>
+  </si>
+  <si>
+    <t>CV</t>
   </si>
 </sst>
 </file>
@@ -493,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,7 +514,7 @@
     <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -524,8 +533,14 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -545,8 +560,14 @@
         <f>(D2+E2)/2</f>
         <v>87.428030540964272</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -566,8 +587,14 @@
         <f t="shared" ref="F3:F9" si="0">(D3+E3)/2</f>
         <v>44.316467587011104</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -587,8 +614,14 @@
         <f t="shared" si="0"/>
         <v>4.7793911729612351</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -608,8 +641,14 @@
         <f t="shared" si="0"/>
         <v>12.937818009651483</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -629,8 +668,14 @@
         <f t="shared" si="0"/>
         <v>386.32036309678693</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -650,8 +695,14 @@
         <f t="shared" si="0"/>
         <v>0.47357657755946347</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -671,8 +722,14 @@
         <f t="shared" si="0"/>
         <v>14.280969368087195</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -691,6 +748,12 @@
       <c r="F9" s="1">
         <f t="shared" si="0"/>
         <v>0.8100095126219865</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revert Param_8 for improved cohort generation in TMDD
</commit_message>
<xml_diff>
--- a/case studies/CaseStudy_TMDD/CaseStudy_TMDD_blank/Param_8.xlsx
+++ b/case studies/CaseStudy_TMDD/CaseStudy_TMDD_blank/Param_8.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feigelmj/Documents/Projects/gQSPsim/release/case studies/CaseStudy_TMDD/CaseStudy_TMDD_complete/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feigelmj\Documents\Projects\gQSPsim\release-v1.1\case studies\CaseStudy_TMDD\CaseStudy_TMDD_blank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A721F44-6614-8842-93EC-360331FCAC20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="1860" windowWidth="25600" windowHeight="16920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="1860" windowWidth="25600" windowHeight="16920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>V1</t>
   </si>
@@ -76,21 +75,12 @@
   </si>
   <si>
     <t>s_target_init</t>
-  </si>
-  <si>
-    <t>Dist</t>
-  </si>
-  <si>
-    <t>norm</t>
-  </si>
-  <si>
-    <t>CV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -501,20 +491,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="9.5" customWidth="1"/>
     <col min="5" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -533,14 +523,8 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -560,14 +544,8 @@
         <f>(D2+E2)/2</f>
         <v>87.428030540964272</v>
       </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -587,14 +565,8 @@
         <f t="shared" ref="F3:F9" si="0">(D3+E3)/2</f>
         <v>44.316467587011104</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -614,14 +586,8 @@
         <f t="shared" si="0"/>
         <v>4.7793911729612351</v>
       </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -641,14 +607,8 @@
         <f t="shared" si="0"/>
         <v>12.937818009651483</v>
       </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -668,14 +628,8 @@
         <f t="shared" si="0"/>
         <v>386.32036309678693</v>
       </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -695,14 +649,8 @@
         <f t="shared" si="0"/>
         <v>0.47357657755946347</v>
       </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -722,14 +670,8 @@
         <f t="shared" si="0"/>
         <v>14.280969368087195</v>
       </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -748,12 +690,6 @@
       <c r="F9" s="1">
         <f t="shared" si="0"/>
         <v>0.8100095126219865</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9">
-        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>